<commit_message>
new datas in .xlsx
</commit_message>
<xml_diff>
--- a/ClassMonitor_Halo/datas/Halo.xlsx
+++ b/ClassMonitor_Halo/datas/Halo.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="8">
   <si>
     <t>min</t>
   </si>
@@ -278,23 +278,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="93598080"/>
-        <c:axId val="93599616"/>
+        <c:axId val="78539776"/>
+        <c:axId val="78542336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="93598080"/>
+        <c:axId val="78539776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93599616"/>
+        <c:crossAx val="78542336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93599616"/>
+        <c:axId val="78542336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -302,7 +302,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93598080"/>
+        <c:crossAx val="78539776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -315,7 +315,238 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="fr-BE"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Heal Normal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$28:$K$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$L$28:$L$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.30104554336500167</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.47647748499104925</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.58968939431550493</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75811393531654803</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5140196403597255</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.1470132971802824</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2235866340027055</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2323765671256881</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.5158516017674799</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.34345558546433</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Heal critical</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$K$28:$K$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$M$28:$M$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.30512979798506595</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.49484545921573553</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.63103671182759313</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.7742208564039551</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.635987358964009</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2109160219257711</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3284557011073801</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3773883107416356</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="56324864"/>
+        <c:axId val="56511488"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="56324864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="56511488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="56511488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="56324864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -348,6 +579,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -641,10 +902,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1189,7 +1450,7 @@
         <v>9.0594309511175997</v>
       </c>
       <c r="G16">
-        <f t="shared" ref="G16:G23" si="6">IF(C16 = 0, 0, D16/C16)</f>
+        <f t="shared" ref="G16:G22" si="6">IF(C16 = 0, 0, D16/C16)</f>
         <v>1.2841798981907917</v>
       </c>
       <c r="H16">
@@ -1509,12 +1770,864 @@
         <v>2.4714062906160601</v>
       </c>
     </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="K26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>3</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>1173</v>
+      </c>
+      <c r="D28">
+        <v>353.12642236714697</v>
+      </c>
+      <c r="E28">
+        <v>182</v>
+      </c>
+      <c r="F28">
+        <v>111.067246466564</v>
+      </c>
+      <c r="G28">
+        <f>IF(C28 = 0, 0, D28/C28)</f>
+        <v>0.30104554336500167</v>
+      </c>
+      <c r="H28">
+        <f>IF(E28 = 0, 0, F28/E28)</f>
+        <v>0.61025959597013191</v>
+      </c>
+      <c r="I28">
+        <f>H28/2</f>
+        <v>0.30512979798506595</v>
+      </c>
+      <c r="K28">
+        <f>AVERAGE(A28,B28)</f>
+        <v>2.5</v>
+      </c>
+      <c r="L28">
+        <f>G28</f>
+        <v>0.30104554336500167</v>
+      </c>
+      <c r="M28">
+        <f>I28</f>
+        <v>0.30512979798506595</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>8</v>
+      </c>
+      <c r="C29">
+        <v>1421</v>
+      </c>
+      <c r="D29">
+        <v>677.07450617228096</v>
+      </c>
+      <c r="E29">
+        <v>208</v>
+      </c>
+      <c r="F29">
+        <v>205.85571103374599</v>
+      </c>
+      <c r="G29">
+        <f t="shared" ref="G29:G38" si="12">IF(C29 = 0, 0, D29/C29)</f>
+        <v>0.47647748499104925</v>
+      </c>
+      <c r="H29">
+        <f t="shared" ref="H29:H38" si="13">IF(E29 = 0, 0, F29/E29)</f>
+        <v>0.98969091843147106</v>
+      </c>
+      <c r="I29">
+        <f t="shared" ref="I29:I38" si="14">H29/2</f>
+        <v>0.49484545921573553</v>
+      </c>
+      <c r="K29">
+        <f t="shared" ref="K29:K38" si="15">AVERAGE(A29,B29)</f>
+        <v>6.5</v>
+      </c>
+      <c r="L29">
+        <f t="shared" ref="L29:L38" si="16">G29</f>
+        <v>0.47647748499104925</v>
+      </c>
+      <c r="M29">
+        <f t="shared" ref="M29:M38" si="17">I29</f>
+        <v>0.49484545921573553</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30">
+        <v>8</v>
+      </c>
+      <c r="B30">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>616</v>
+      </c>
+      <c r="D30">
+        <v>363.24866689835102</v>
+      </c>
+      <c r="E30">
+        <v>102</v>
+      </c>
+      <c r="F30">
+        <v>128.73148921282899</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="12"/>
+        <v>0.58968939431550493</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="13"/>
+        <v>1.2620734236551863</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="14"/>
+        <v>0.63103671182759313</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="15"/>
+        <v>9</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="16"/>
+        <v>0.58968939431550493</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="17"/>
+        <v>0.63103671182759313</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31">
+        <v>10</v>
+      </c>
+      <c r="B31">
+        <v>15</v>
+      </c>
+      <c r="C31">
+        <v>1967</v>
+      </c>
+      <c r="D31">
+        <v>1491.2101107676499</v>
+      </c>
+      <c r="E31">
+        <v>301</v>
+      </c>
+      <c r="F31">
+        <v>466.08095555518099</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="12"/>
+        <v>0.75811393531654803</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="13"/>
+        <v>1.5484417128079102</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="14"/>
+        <v>0.7742208564039551</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="15"/>
+        <v>12.5</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="16"/>
+        <v>0.75811393531654803</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="17"/>
+        <v>0.7742208564039551</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32">
+        <v>15</v>
+      </c>
+      <c r="B32">
+        <v>20</v>
+      </c>
+      <c r="C32">
+        <v>2185</v>
+      </c>
+      <c r="D32">
+        <v>3308.1329141860001</v>
+      </c>
+      <c r="E32">
+        <v>328</v>
+      </c>
+      <c r="F32">
+        <v>1073.2077074803899</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="12"/>
+        <v>1.5140196403597255</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="13"/>
+        <v>3.2719747179280181</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="14"/>
+        <v>1.635987358964009</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="15"/>
+        <v>17.5</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="16"/>
+        <v>1.5140196403597255</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="17"/>
+        <v>1.635987358964009</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33">
+        <v>20</v>
+      </c>
+      <c r="B33">
+        <v>25</v>
+      </c>
+      <c r="C33">
+        <v>1912</v>
+      </c>
+      <c r="D33">
+        <v>4105.0894242086997</v>
+      </c>
+      <c r="E33">
+        <v>266</v>
+      </c>
+      <c r="F33">
+        <v>1176.2073236645101</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="12"/>
+        <v>2.1470132971802824</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="13"/>
+        <v>4.4218320438515422</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="14"/>
+        <v>2.2109160219257711</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="15"/>
+        <v>22.5</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="16"/>
+        <v>2.1470132971802824</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="17"/>
+        <v>2.2109160219257711</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34">
+        <v>25</v>
+      </c>
+      <c r="B34">
+        <v>30</v>
+      </c>
+      <c r="C34">
+        <v>913</v>
+      </c>
+      <c r="D34">
+        <v>2030.13459684447</v>
+      </c>
+      <c r="E34">
+        <v>142</v>
+      </c>
+      <c r="F34">
+        <v>661.28141911449598</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="12"/>
+        <v>2.2235866340027055</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="13"/>
+        <v>4.6569114022147602</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="14"/>
+        <v>2.3284557011073801</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="15"/>
+        <v>27.5</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="16"/>
+        <v>2.2235866340027055</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="17"/>
+        <v>2.3284557011073801</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <v>35</v>
+      </c>
+      <c r="C35">
+        <v>141</v>
+      </c>
+      <c r="D35">
+        <v>173.76509596472201</v>
+      </c>
+      <c r="E35">
+        <v>31</v>
+      </c>
+      <c r="F35">
+        <v>85.398075265981404</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="12"/>
+        <v>1.2323765671256881</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="13"/>
+        <v>2.7547766214832712</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="14"/>
+        <v>1.3773883107416356</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="15"/>
+        <v>32.5</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="16"/>
+        <v>1.2323765671256881</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="17"/>
+        <v>1.3773883107416356</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>40</v>
+      </c>
+      <c r="C36">
+        <v>5</v>
+      </c>
+      <c r="D36">
+        <v>17.5792580088374</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="12"/>
+        <v>3.5158516017674799</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="15"/>
+        <v>37.5</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="16"/>
+        <v>3.5158516017674799</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37">
+        <v>40</v>
+      </c>
+      <c r="B37">
+        <v>45</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>4.6869111709286599</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="12"/>
+        <v>2.34345558546433</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="15"/>
+        <v>42.5</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="16"/>
+        <v>2.34345558546433</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38">
+        <v>9</v>
+      </c>
+      <c r="B38">
+        <v>28</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="15"/>
+        <v>18.5</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <v>42</v>
+      </c>
+      <c r="D41">
+        <v>36.017225747308402</v>
+      </c>
+      <c r="E41">
+        <v>7</v>
+      </c>
+      <c r="F41">
+        <v>17.3382879933793</v>
+      </c>
+      <c r="G41">
+        <f t="shared" ref="G41:G47" si="18">IF(C41 = 0, 0, D41/C41)</f>
+        <v>0.85755299398353335</v>
+      </c>
+      <c r="H41">
+        <f t="shared" ref="H41:H48" si="19">IF(E41 = 0, 0, F41/E41)</f>
+        <v>2.4768982847684713</v>
+      </c>
+      <c r="I41">
+        <f t="shared" ref="I41:I48" si="20">H41/2</f>
+        <v>1.2384491423842356</v>
+      </c>
+      <c r="K41">
+        <f t="shared" ref="K41:K48" si="21">AVERAGE(A41,B41)</f>
+        <v>2.5</v>
+      </c>
+      <c r="L41">
+        <f t="shared" ref="L41:L48" si="22">G41</f>
+        <v>0.85755299398353335</v>
+      </c>
+      <c r="M41">
+        <f t="shared" ref="M41:M48" si="23">I41</f>
+        <v>1.2384491423842356</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>8</v>
+      </c>
+      <c r="C42">
+        <v>77</v>
+      </c>
+      <c r="D42">
+        <v>118.05578442135899</v>
+      </c>
+      <c r="E42">
+        <v>11</v>
+      </c>
+      <c r="F42">
+        <v>33.992727810156502</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="18"/>
+        <v>1.5331920054721948</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="19"/>
+        <v>3.0902479827415004</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="20"/>
+        <v>1.5451239913707502</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="21"/>
+        <v>6.5</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="22"/>
+        <v>1.5331920054721948</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="23"/>
+        <v>1.5451239913707502</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43">
+        <v>8</v>
+      </c>
+      <c r="B43">
+        <v>10</v>
+      </c>
+      <c r="C43">
+        <v>26</v>
+      </c>
+      <c r="D43">
+        <v>43.335399263470798</v>
+      </c>
+      <c r="E43">
+        <v>4</v>
+      </c>
+      <c r="F43">
+        <v>13.9313964877957</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="18"/>
+        <v>1.6667461255181075</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="19"/>
+        <v>3.482849121948925</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="20"/>
+        <v>1.7414245609744625</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="22"/>
+        <v>1.6667461255181075</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="23"/>
+        <v>1.7414245609744625</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44">
+        <v>10</v>
+      </c>
+      <c r="B44">
+        <v>15</v>
+      </c>
+      <c r="C44">
+        <v>101</v>
+      </c>
+      <c r="D44">
+        <v>252.03617110486601</v>
+      </c>
+      <c r="E44">
+        <v>14</v>
+      </c>
+      <c r="F44">
+        <v>67.711599450143495</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="18"/>
+        <v>2.4954076347016438</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="19"/>
+        <v>4.8365428178673922</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="20"/>
+        <v>2.4182714089336961</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="21"/>
+        <v>12.5</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="22"/>
+        <v>2.4954076347016438</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="23"/>
+        <v>2.4182714089336961</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45">
+        <v>15</v>
+      </c>
+      <c r="B45">
+        <v>20</v>
+      </c>
+      <c r="C45">
+        <v>92</v>
+      </c>
+      <c r="D45">
+        <v>308.99427882713201</v>
+      </c>
+      <c r="E45">
+        <v>14</v>
+      </c>
+      <c r="F45">
+        <v>98.064287716630901</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="18"/>
+        <v>3.3586334655123045</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="19"/>
+        <v>7.0045919797593497</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="20"/>
+        <v>3.5022959898796748</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="21"/>
+        <v>17.5</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="22"/>
+        <v>3.3586334655123045</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="23"/>
+        <v>3.5022959898796748</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46">
+        <v>20</v>
+      </c>
+      <c r="B46">
+        <v>25</v>
+      </c>
+      <c r="C46">
+        <v>79</v>
+      </c>
+      <c r="D46">
+        <v>253.92478923377999</v>
+      </c>
+      <c r="E46">
+        <v>8</v>
+      </c>
+      <c r="F46">
+        <v>55.075415297926</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="18"/>
+        <v>3.2142378384022785</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="19"/>
+        <v>6.88442691224075</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="20"/>
+        <v>3.442213456120375</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="21"/>
+        <v>22.5</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="22"/>
+        <v>3.2142378384022785</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="23"/>
+        <v>3.442213456120375</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47">
+        <v>25</v>
+      </c>
+      <c r="B47">
+        <v>30</v>
+      </c>
+      <c r="C47">
+        <v>27</v>
+      </c>
+      <c r="D47">
+        <v>74.669098124569302</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="18"/>
+        <v>2.7655221527618261</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="21"/>
+        <v>27.5</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="22"/>
+        <v>2.7655221527618261</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48">
+        <v>30</v>
+      </c>
+      <c r="B48">
+        <v>35</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>4.9428125812321202</v>
+      </c>
+      <c r="G48">
+        <f>IF(C48 = 0, 0, D48/C48)</f>
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="19"/>
+        <v>4.9428125812321202</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="20"/>
+        <v>2.4714062906160601</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="21"/>
+        <v>32.5</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="23"/>
+        <v>2.4714062906160601</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="K1:M1"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="K26:M26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>